<commit_message>
V1 script merging done
</commit_message>
<xml_diff>
--- a/Inputs/Cigna/benefits.xlsx
+++ b/Inputs/Cigna/benefits.xlsx
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Out-patient (Consultations, Lab &amp; Diagnostics, Pharmacy, Physiotherapy)</t>
   </si>
   <si>
-    <t xml:space="preserve">Out-patient benefits </t>
+    <t xml:space="preserve">Out-patient benefits</t>
   </si>
   <si>
     <t xml:space="preserve">Medicines and diagnostics &amp; lab tests covered in full 
@@ -982,11 +982,11 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.04"/>
@@ -3774,7 +3774,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="10.4"/>
   </cols>

</xml_diff>